<commit_message>
Update BOM with regional data
</commit_message>
<xml_diff>
--- a/Assembly Guide/Bill_of_Materials.xlsx
+++ b/Assembly Guide/Bill_of_Materials.xlsx
@@ -8,7 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="USA" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Europe" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Asia" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="52">
   <si>
     <t xml:space="preserve">PRODUCT NUMBER</t>
   </si>
@@ -149,6 +151,33 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.adafruit.com/product/3157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qualatex Round Microfoil Balloon: 36’’ Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~2.5 USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qualatex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer to Alt Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://us.qualatex.com/en-us/products/12683/?product_type=Qualatex%20Foil%20Balloons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://europe.qualatex.com/en-gb/products/12683/?product_type=Qualatex%20Foil%20Balloons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://europe.qualatex.com/en-gb/purchase-qualatex-balloons/europe-distributors/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://asia.qualatex.com/en-us/products/12683/?product_type=Qualatex%20Foil%20Balloons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://asia.qualatex.com/en-us/purchase-qualatex-balloons/asia-distributors/</t>
   </si>
 </sst>
 </file>
@@ -344,10 +373,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -631,7 +660,35 @@
       </c>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>12683</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -642,4 +699,672 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="30.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="11.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>3400</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>1578</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1903</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2135</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>2990</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>3099</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <v>3157</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>12683</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="30.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="11.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>3400</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>1578</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1903</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2135</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>2990</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>3099</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <v>3157</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>12683</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>